<commit_message>
update cases run status
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/cases_info.xlsx
+++ b/use_cases/SMR_FT_2023/data/cases_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD4A70-206D-5540-B954-5CE7AFBC7333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCF4BA0-A4DD-CF4C-B495-8085860FCD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="1440" windowWidth="31160" windowHeight="17880" activeTab="1" xr2:uid="{9C68323A-2460-E743-B5FC-B455388DAB58}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
   <si>
     <t>Plant</t>
   </si>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,19 +1063,19 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1109,19 +1109,19 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
         <v>70</v>
@@ -1137,37 +1137,25 @@
       <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1175,19 +1163,19 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1197,17 +1185,14 @@
       <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1215,19 +1200,16 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1235,19 +1217,13 @@
         <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1255,19 +1231,19 @@
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1275,19 +1251,13 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1295,19 +1265,13 @@
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1315,19 +1279,19 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1335,19 +1299,16 @@
         <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1355,19 +1316,19 @@
         <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1378,16 +1339,16 @@
         <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1398,16 +1359,13 @@
         <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>